<commit_message>
≡ƒÜÇ PO Status update via batch
</commit_message>
<xml_diff>
--- a/po-status.xlsx
+++ b/po-status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esolon\OneDrive - Boston Semi Equipment LLC\Github Projects\PO_Status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mvtstechnologies-my.sharepoint.com/personal/edsel_solon_bsegroup_com/Documents/Github Projects/PO_Status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52648CD9-9588-495C-B516-DCF04B27A16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_BEA61AB93885F3985D2921609675981670D885A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E181D362-08B5-4B8B-A92D-57A72A7E0BB3}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
     <t>TBA</t>
   </si>
   <si>
-    <t>Last updated: 2025-07-14 07:59:41</t>
+    <t>Last updated: 2025-07-15 06:10:51</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>16</v>
@@ -714,10 +714,10 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1012,7 +1012,7 @@
         <v>41</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>14</v>
@@ -1024,10 +1024,10 @@
         <v>14</v>
       </c>
       <c r="H20">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>